<commit_message>
corrected calcul of indicators from history
</commit_message>
<xml_diff>
--- a/risk_indicators.xlsx
+++ b/risk_indicators.xlsx
@@ -865,7 +865,7 @@
       </c>
       <c r="E7" s="11" t="n"/>
       <c r="F7" s="6" t="n">
-        <v>0.991304347826087</v>
+        <v>1</v>
       </c>
       <c r="G7" s="10" t="n">
         <v>1</v>
@@ -879,10 +879,10 @@
       </c>
       <c r="K7" s="11" t="n"/>
       <c r="L7" s="6" t="n">
-        <v>0.6185344827586207</v>
+        <v>0.1443965517241379</v>
       </c>
       <c r="M7" s="10" t="n">
-        <v>0.7607758620689655</v>
+        <v>0.2866379310344828</v>
       </c>
       <c r="N7" s="11" t="n"/>
     </row>
@@ -900,10 +900,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.303921568627451</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>18</v>
@@ -932,10 +932,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="I9" t="n">
         <v>18</v>
@@ -1038,10 +1038,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
         <v>18</v>
@@ -1050,10 +1050,10 @@
         <v>18</v>
       </c>
       <c r="L12" t="n">
-        <v>0.4859154929577465</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>0.443661971830986</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1070,10 +1070,10 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>18</v>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E15" s="11" t="n"/>
       <c r="F15" s="6" t="n">
-        <v>1</v>
+        <v>0.6349206349206349</v>
       </c>
       <c r="G15" s="10" t="n">
         <v>1</v>
@@ -1176,10 +1176,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
         <v>18</v>
@@ -1188,10 +1188,10 @@
         <v>18</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1208,10 +1208,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
         <v>18</v>
@@ -1220,10 +1220,10 @@
         <v>18</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -1241,10 +1241,10 @@
       </c>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="7" t="n">
-        <v>0.04761904761904767</v>
+        <v>0</v>
       </c>
       <c r="G18" s="8" t="n">
-        <v>0.04761904761904767</v>
+        <v>0</v>
       </c>
       <c r="H18" s="9" t="n"/>
       <c r="I18" s="7" t="n">
@@ -1279,10 +1279,10 @@
       </c>
       <c r="E19" s="11" t="n"/>
       <c r="F19" s="6" t="n">
-        <v>1</v>
+        <v>0.5280898876404494</v>
       </c>
       <c r="G19" s="10" t="n">
-        <v>1</v>
+        <v>0.4157303370786517</v>
       </c>
       <c r="H19" s="11" t="n"/>
       <c r="I19" s="6" t="n">
@@ -1314,10 +1314,10 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>18</v>
@@ -1326,10 +1326,10 @@
         <v>18</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1346,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
         <v>18</v>
@@ -1358,10 +1358,10 @@
         <v>18</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -1379,10 +1379,10 @@
       </c>
       <c r="E22" s="9" t="n"/>
       <c r="F22" s="7" t="n">
-        <v>0.7894736842105263</v>
+        <v>0</v>
       </c>
       <c r="G22" s="8" t="n">
-        <v>0.7894736842105263</v>
+        <v>0</v>
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="7" t="n">
@@ -1417,10 +1417,10 @@
       </c>
       <c r="E23" s="11" t="n"/>
       <c r="F23" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="11" t="n"/>
       <c r="I23" s="6" t="n">
@@ -1431,10 +1431,10 @@
       </c>
       <c r="K23" s="11" t="n"/>
       <c r="L23" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="11" t="n"/>
     </row>
@@ -1452,10 +1452,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
         <v>18</v>
@@ -1464,10 +1464,10 @@
         <v>18</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1484,10 +1484,10 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
         <v>18</v>
@@ -1496,10 +1496,10 @@
         <v>18</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -1517,10 +1517,10 @@
       </c>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="9" t="n"/>
       <c r="I26" s="7" t="n">
@@ -1555,10 +1555,10 @@
       </c>
       <c r="E27" s="11" t="n"/>
       <c r="F27" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="11" t="n"/>
       <c r="I27" s="6" t="n">
@@ -1569,10 +1569,10 @@
       </c>
       <c r="K27" s="11" t="n"/>
       <c r="L27" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="11" t="n"/>
     </row>
@@ -1590,10 +1590,10 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
         <v>18</v>
@@ -1602,10 +1602,10 @@
         <v>18</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1622,10 +1622,10 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
         <v>18</v>
@@ -1634,10 +1634,10 @@
         <v>18</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -1655,10 +1655,10 @@
       </c>
       <c r="E30" s="9" t="n"/>
       <c r="F30" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="9" t="n"/>
       <c r="I30" s="7" t="n">
@@ -1693,10 +1693,10 @@
       </c>
       <c r="E31" s="11" t="n"/>
       <c r="F31" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="11" t="n"/>
       <c r="I31" s="6" t="n">
@@ -1707,10 +1707,10 @@
       </c>
       <c r="K31" s="11" t="n"/>
       <c r="L31" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="11" t="n"/>
     </row>
@@ -1728,10 +1728,10 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
         <v>18</v>
@@ -1740,10 +1740,10 @@
         <v>18</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1760,10 +1760,10 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="n">
         <v>18</v>
@@ -1772,10 +1772,10 @@
         <v>18</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -1793,10 +1793,10 @@
       </c>
       <c r="E34" s="9" t="n"/>
       <c r="F34" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="9" t="n"/>
       <c r="I34" s="7" t="n">
@@ -1831,10 +1831,10 @@
       </c>
       <c r="E35" s="11" t="n"/>
       <c r="F35" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="11" t="n"/>
       <c r="I35" s="6" t="n">
@@ -1845,10 +1845,10 @@
       </c>
       <c r="K35" s="11" t="n"/>
       <c r="L35" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="11" t="n"/>
     </row>
@@ -1866,10 +1866,10 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
         <v>18</v>
@@ -1878,10 +1878,10 @@
         <v>18</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1898,10 +1898,10 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
         <v>18</v>
@@ -1910,10 +1910,10 @@
         <v>18</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -1931,10 +1931,10 @@
       </c>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="9" t="n"/>
       <c r="I38" s="7" t="n">
@@ -1969,10 +1969,10 @@
       </c>
       <c r="E39" s="11" t="n"/>
       <c r="F39" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="11" t="n"/>
       <c r="I39" s="6" t="n">
@@ -1983,10 +1983,10 @@
       </c>
       <c r="K39" s="11" t="n"/>
       <c r="L39" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39" s="11" t="n"/>
     </row>
@@ -2004,10 +2004,10 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
         <v>18</v>
@@ -2016,10 +2016,10 @@
         <v>18</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -2036,10 +2036,10 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
         <v>18</v>
@@ -2048,10 +2048,10 @@
         <v>18</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -2069,10 +2069,10 @@
       </c>
       <c r="E42" s="9" t="n"/>
       <c r="F42" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="9" t="n"/>
       <c r="I42" s="7" t="n">
@@ -2107,10 +2107,10 @@
       </c>
       <c r="E43" s="11" t="n"/>
       <c r="F43" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="11" t="n"/>
       <c r="I43" s="6" t="n">
@@ -2121,10 +2121,10 @@
       </c>
       <c r="K43" s="11" t="n"/>
       <c r="L43" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M43" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N43" s="11" t="n"/>
     </row>
@@ -2142,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
@@ -2154,10 +2154,10 @@
         <v>18</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -2174,10 +2174,10 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
         <v>18</v>
@@ -2186,10 +2186,10 @@
         <v>18</v>
       </c>
       <c r="L45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -2207,10 +2207,10 @@
       </c>
       <c r="E46" s="9" t="n"/>
       <c r="F46" s="7" t="n">
-        <v>0.3103448275862069</v>
+        <v>0</v>
       </c>
       <c r="G46" s="8" t="n">
-        <v>0.2413793103448276</v>
+        <v>0</v>
       </c>
       <c r="H46" s="9" t="n"/>
       <c r="I46" s="7" t="n">
@@ -2245,10 +2245,10 @@
       </c>
       <c r="E47" s="11" t="n"/>
       <c r="F47" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" s="11" t="n"/>
       <c r="I47" s="6" t="n">
@@ -2259,10 +2259,10 @@
       </c>
       <c r="K47" s="11" t="n"/>
       <c r="L47" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N47" s="11" t="n"/>
     </row>
@@ -2280,10 +2280,10 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
         <v>18</v>
@@ -2292,10 +2292,10 @@
         <v>18</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2312,10 +2312,10 @@
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" t="n">
         <v>18</v>
@@ -2324,10 +2324,10 @@
         <v>18</v>
       </c>
       <c r="L49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -2383,10 +2383,10 @@
       </c>
       <c r="E51" s="11" t="n"/>
       <c r="F51" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" s="11" t="n"/>
       <c r="I51" s="6" t="n">
@@ -2397,10 +2397,10 @@
       </c>
       <c r="K51" s="11" t="n"/>
       <c r="L51" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N51" s="11" t="n"/>
     </row>
@@ -2418,10 +2418,10 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
         <v>18</v>
@@ -2430,10 +2430,10 @@
         <v>18</v>
       </c>
       <c r="L52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -2450,10 +2450,10 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="n">
         <v>18</v>
@@ -2462,10 +2462,10 @@
         <v>18</v>
       </c>
       <c r="L53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="E55" s="11" t="n"/>
       <c r="F55" s="6" t="n">
-        <v>1</v>
+        <v>0.5833333333333333</v>
       </c>
       <c r="G55" s="10" t="n">
         <v>1</v>
@@ -2535,10 +2535,10 @@
       </c>
       <c r="K55" s="11" t="n"/>
       <c r="L55" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M55" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N55" s="11" t="n"/>
     </row>
@@ -2556,10 +2556,10 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="n">
         <v>18</v>
@@ -2568,10 +2568,10 @@
         <v>18</v>
       </c>
       <c r="L56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2588,10 +2588,10 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
         <v>18</v>
@@ -2600,10 +2600,10 @@
         <v>18</v>
       </c>
       <c r="L57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="E59" s="11" t="n"/>
       <c r="F59" s="6" t="n">
-        <v>1</v>
+        <v>0.6451612903225838</v>
       </c>
       <c r="G59" s="10" t="n">
         <v>1</v>
@@ -2673,10 +2673,10 @@
       </c>
       <c r="K59" s="11" t="n"/>
       <c r="L59" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M59" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N59" s="11" t="n"/>
     </row>
@@ -2694,10 +2694,10 @@
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="n">
         <v>18</v>
@@ -2706,10 +2706,10 @@
         <v>18</v>
       </c>
       <c r="L60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2726,10 +2726,10 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="n">
         <v>18</v>
@@ -2738,10 +2738,10 @@
         <v>18</v>
       </c>
       <c r="L61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="E63" s="11" t="n"/>
       <c r="F63" s="6" t="n">
-        <v>1</v>
+        <v>0.6065573770491803</v>
       </c>
       <c r="G63" s="10" t="n">
         <v>1</v>
@@ -2811,10 +2811,10 @@
       </c>
       <c r="K63" s="11" t="n"/>
       <c r="L63" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M63" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N63" s="11" t="n"/>
     </row>
@@ -2832,10 +2832,10 @@
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" t="n">
         <v>18</v>
@@ -2844,10 +2844,10 @@
         <v>18</v>
       </c>
       <c r="L64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2864,10 +2864,10 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="n">
         <v>18</v>
@@ -2876,10 +2876,10 @@
         <v>18</v>
       </c>
       <c r="L65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -2897,10 +2897,10 @@
       </c>
       <c r="E66" s="9" t="n"/>
       <c r="F66" s="7" t="n">
-        <v>0.1153846153846154</v>
+        <v>0</v>
       </c>
       <c r="G66" s="8" t="n">
-        <v>0.04000000000000004</v>
+        <v>0</v>
       </c>
       <c r="H66" s="9" t="n"/>
       <c r="I66" s="7" t="n">
@@ -2935,10 +2935,10 @@
       </c>
       <c r="E67" s="11" t="n"/>
       <c r="F67" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" s="11" t="n"/>
       <c r="I67" s="6" t="n">
@@ -2949,10 +2949,10 @@
       </c>
       <c r="K67" s="11" t="n"/>
       <c r="L67" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M67" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N67" s="11" t="n"/>
     </row>
@@ -2970,10 +2970,10 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="n">
         <v>18</v>
@@ -2982,10 +2982,10 @@
         <v>18</v>
       </c>
       <c r="L68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -3002,10 +3002,10 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="n">
         <v>18</v>
@@ -3014,10 +3014,10 @@
         <v>18</v>
       </c>
       <c r="L69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -3035,10 +3035,10 @@
       </c>
       <c r="E70" s="9" t="n"/>
       <c r="F70" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" s="9" t="n"/>
       <c r="I70" s="7" t="n">
@@ -3073,10 +3073,10 @@
       </c>
       <c r="E71" s="11" t="n"/>
       <c r="F71" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71" s="11" t="n"/>
       <c r="I71" s="6" t="n">
@@ -3087,10 +3087,10 @@
       </c>
       <c r="K71" s="11" t="n"/>
       <c r="L71" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M71" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N71" s="11" t="n"/>
     </row>
@@ -3108,10 +3108,10 @@
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" t="n">
         <v>18</v>
@@ -3120,10 +3120,10 @@
         <v>18</v>
       </c>
       <c r="L72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -3140,10 +3140,10 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" t="n">
         <v>18</v>
@@ -3152,10 +3152,10 @@
         <v>18</v>
       </c>
       <c r="L73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -3173,10 +3173,10 @@
       </c>
       <c r="E74" s="9" t="n"/>
       <c r="F74" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" s="9" t="n"/>
       <c r="I74" s="7" t="n">
@@ -3211,10 +3211,10 @@
       </c>
       <c r="E75" s="11" t="n"/>
       <c r="F75" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75" s="11" t="n"/>
       <c r="I75" s="6" t="n">
@@ -3225,10 +3225,10 @@
       </c>
       <c r="K75" s="11" t="n"/>
       <c r="L75" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M75" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N75" s="11" t="n"/>
     </row>
@@ -3246,10 +3246,10 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" t="n">
         <v>18</v>
@@ -3258,10 +3258,10 @@
         <v>18</v>
       </c>
       <c r="L76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -3278,10 +3278,10 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" t="n">
         <v>18</v>
@@ -3290,10 +3290,10 @@
         <v>18</v>
       </c>
       <c r="L77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -3311,10 +3311,10 @@
       </c>
       <c r="E78" s="9" t="n"/>
       <c r="F78" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78" s="9" t="n"/>
       <c r="I78" s="7" t="n">
@@ -3349,10 +3349,10 @@
       </c>
       <c r="E79" s="11" t="n"/>
       <c r="F79" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" s="11" t="n"/>
       <c r="I79" s="6" t="n">
@@ -3363,10 +3363,10 @@
       </c>
       <c r="K79" s="11" t="n"/>
       <c r="L79" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M79" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N79" s="11" t="n"/>
     </row>
@@ -3384,10 +3384,10 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" t="n">
         <v>18</v>
@@ -3396,10 +3396,10 @@
         <v>18</v>
       </c>
       <c r="L80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -3416,10 +3416,10 @@
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" t="n">
         <v>18</v>
@@ -3428,10 +3428,10 @@
         <v>18</v>
       </c>
       <c r="L81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -3449,10 +3449,10 @@
       </c>
       <c r="E82" s="9" t="n"/>
       <c r="F82" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" s="9" t="n"/>
       <c r="I82" s="7" t="n">
@@ -3487,10 +3487,10 @@
       </c>
       <c r="E83" s="11" t="n"/>
       <c r="F83" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" s="11" t="n"/>
       <c r="I83" s="6" t="n">
@@ -3501,10 +3501,10 @@
       </c>
       <c r="K83" s="11" t="n"/>
       <c r="L83" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M83" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N83" s="11" t="n"/>
     </row>
@@ -3522,10 +3522,10 @@
         <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="n">
         <v>18</v>
@@ -3534,10 +3534,10 @@
         <v>18</v>
       </c>
       <c r="L84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -3554,10 +3554,10 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85" t="n">
         <v>18</v>
@@ -3566,10 +3566,10 @@
         <v>18</v>
       </c>
       <c r="L85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -3587,10 +3587,10 @@
       </c>
       <c r="E86" s="9" t="n"/>
       <c r="F86" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G86" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86" s="9" t="n"/>
       <c r="I86" s="7" t="n">
@@ -3625,10 +3625,10 @@
       </c>
       <c r="E87" s="11" t="n"/>
       <c r="F87" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87" s="11" t="n"/>
       <c r="I87" s="6" t="n">
@@ -3639,10 +3639,10 @@
       </c>
       <c r="K87" s="11" t="n"/>
       <c r="L87" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M87" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N87" s="11" t="n"/>
     </row>
@@ -3660,10 +3660,10 @@
         <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" t="n">
         <v>18</v>
@@ -3672,10 +3672,10 @@
         <v>18</v>
       </c>
       <c r="L88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3692,10 +3692,10 @@
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" t="n">
         <v>18</v>
@@ -3704,10 +3704,10 @@
         <v>18</v>
       </c>
       <c r="L89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -3725,10 +3725,10 @@
       </c>
       <c r="E90" s="9" t="n"/>
       <c r="F90" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90" s="9" t="n"/>
       <c r="I90" s="7" t="n">
@@ -3763,10 +3763,10 @@
       </c>
       <c r="E91" s="11" t="n"/>
       <c r="F91" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91" s="11" t="n"/>
       <c r="I91" s="6" t="n">
@@ -3777,10 +3777,10 @@
       </c>
       <c r="K91" s="11" t="n"/>
       <c r="L91" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M91" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N91" s="11" t="n"/>
     </row>
@@ -3798,10 +3798,10 @@
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92" t="n">
         <v>18</v>
@@ -3810,10 +3810,10 @@
         <v>18</v>
       </c>
       <c r="L92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -3830,10 +3830,10 @@
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" t="n">
         <v>18</v>
@@ -3842,10 +3842,10 @@
         <v>18</v>
       </c>
       <c r="L93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -3863,10 +3863,10 @@
       </c>
       <c r="E94" s="9" t="n"/>
       <c r="F94" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G94" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94" s="9" t="n"/>
       <c r="I94" s="7" t="n">
@@ -3901,10 +3901,10 @@
       </c>
       <c r="E95" s="11" t="n"/>
       <c r="F95" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G95" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95" s="11" t="n"/>
       <c r="I95" s="6" t="n">
@@ -3915,10 +3915,10 @@
       </c>
       <c r="K95" s="11" t="n"/>
       <c r="L95" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M95" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N95" s="11" t="n"/>
     </row>
@@ -3936,10 +3936,10 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="n">
         <v>18</v>
@@ -3948,10 +3948,10 @@
         <v>18</v>
       </c>
       <c r="L96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -3968,10 +3968,10 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" t="n">
         <v>18</v>
@@ -3980,10 +3980,10 @@
         <v>18</v>
       </c>
       <c r="L97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -4001,10 +4001,10 @@
       </c>
       <c r="E98" s="9" t="n"/>
       <c r="F98" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98" s="9" t="n"/>
       <c r="I98" s="7" t="n">
@@ -4039,10 +4039,10 @@
       </c>
       <c r="E99" s="11" t="n"/>
       <c r="F99" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G99" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" s="11" t="n"/>
       <c r="I99" s="6" t="n">
@@ -4053,10 +4053,10 @@
       </c>
       <c r="K99" s="11" t="n"/>
       <c r="L99" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M99" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N99" s="11" t="n"/>
     </row>
@@ -4074,10 +4074,10 @@
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100" t="n">
         <v>18</v>
@@ -4086,10 +4086,10 @@
         <v>18</v>
       </c>
       <c r="L100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -4106,10 +4106,10 @@
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" t="n">
         <v>18</v>
@@ -4118,10 +4118,10 @@
         <v>18</v>
       </c>
       <c r="L101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -4139,10 +4139,10 @@
       </c>
       <c r="E102" s="9" t="n"/>
       <c r="F102" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G102" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102" s="9" t="n"/>
       <c r="I102" s="7" t="n">
@@ -4177,10 +4177,10 @@
       </c>
       <c r="E103" s="11" t="n"/>
       <c r="F103" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G103" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H103" s="11" t="n"/>
       <c r="I103" s="6" t="n">
@@ -4191,10 +4191,10 @@
       </c>
       <c r="K103" s="11" t="n"/>
       <c r="L103" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M103" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N103" s="11" t="n"/>
     </row>
@@ -4212,10 +4212,10 @@
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104" t="n">
         <v>18</v>
@@ -4224,10 +4224,10 @@
         <v>18</v>
       </c>
       <c r="L104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -4244,10 +4244,10 @@
         <v>0</v>
       </c>
       <c r="F105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105" t="n">
         <v>18</v>
@@ -4256,10 +4256,10 @@
         <v>18</v>
       </c>
       <c r="L105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -4277,10 +4277,10 @@
       </c>
       <c r="E106" s="9" t="n"/>
       <c r="F106" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G106" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H106" s="9" t="n"/>
       <c r="I106" s="7" t="n">
@@ -4329,10 +4329,10 @@
       </c>
       <c r="K107" s="11" t="n"/>
       <c r="L107" s="6" t="n">
-        <v>0</v>
+        <v>0.9341692789968652</v>
       </c>
       <c r="M107" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N107" s="11" t="n"/>
     </row>
@@ -4350,10 +4350,10 @@
         <v>0</v>
       </c>
       <c r="F108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I108" t="n">
         <v>18</v>
@@ -4362,10 +4362,10 @@
         <v>18</v>
       </c>
       <c r="L108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -4382,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="F109" t="n">
-        <v>1</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="G109" t="n">
         <v>1</v>
@@ -4394,10 +4394,10 @@
         <v>18</v>
       </c>
       <c r="L109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -4415,10 +4415,10 @@
       </c>
       <c r="E110" s="9" t="n"/>
       <c r="F110" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G110" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H110" s="9" t="n"/>
       <c r="I110" s="7" t="n">
@@ -4467,10 +4467,10 @@
       </c>
       <c r="K111" s="11" t="n"/>
       <c r="L111" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M111" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N111" s="11" t="n"/>
     </row>
@@ -4488,10 +4488,10 @@
         <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I112" t="n">
         <v>18</v>
@@ -4500,10 +4500,10 @@
         <v>18</v>
       </c>
       <c r="L112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -4520,10 +4520,10 @@
         <v>0</v>
       </c>
       <c r="F113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I113" t="n">
         <v>18</v>
@@ -4532,10 +4532,10 @@
         <v>18</v>
       </c>
       <c r="L113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -4553,10 +4553,10 @@
       </c>
       <c r="E114" s="9" t="n"/>
       <c r="F114" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G114" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H114" s="9" t="n"/>
       <c r="I114" s="7" t="n">
@@ -4567,7 +4567,7 @@
       </c>
       <c r="K114" s="9" t="n"/>
       <c r="L114" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M114" s="8" t="n">
         <v>1</v>
@@ -4605,10 +4605,10 @@
       </c>
       <c r="K115" s="11" t="n"/>
       <c r="L115" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M115" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N115" s="11" t="n"/>
     </row>
@@ -4626,10 +4626,10 @@
         <v>0</v>
       </c>
       <c r="F116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I116" t="n">
         <v>18</v>
@@ -4638,10 +4638,10 @@
         <v>18</v>
       </c>
       <c r="L116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -4658,10 +4658,10 @@
         <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I117" t="n">
         <v>18</v>
@@ -4670,10 +4670,10 @@
         <v>18</v>
       </c>
       <c r="L117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -4691,10 +4691,10 @@
       </c>
       <c r="E118" s="9" t="n"/>
       <c r="F118" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G118" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H118" s="9" t="n"/>
       <c r="I118" s="7" t="n">
@@ -4705,10 +4705,10 @@
       </c>
       <c r="K118" s="9" t="n"/>
       <c r="L118" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M118" s="8" t="n">
-        <v>0.9428571428571428</v>
+        <v>1</v>
       </c>
       <c r="N118" s="9" t="n"/>
     </row>
@@ -4729,7 +4729,7 @@
       </c>
       <c r="E119" s="11" t="n"/>
       <c r="F119" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G119" s="10" t="n">
         <v>1</v>
@@ -4743,10 +4743,10 @@
       </c>
       <c r="K119" s="11" t="n"/>
       <c r="L119" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M119" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N119" s="11" t="n"/>
     </row>
@@ -4764,10 +4764,10 @@
         <v>0</v>
       </c>
       <c r="F120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I120" t="n">
         <v>18</v>
@@ -4776,10 +4776,10 @@
         <v>18</v>
       </c>
       <c r="L120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -4796,10 +4796,10 @@
         <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" t="n">
         <v>18</v>
@@ -4808,10 +4808,10 @@
         <v>18</v>
       </c>
       <c r="L121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -4829,10 +4829,10 @@
       </c>
       <c r="E122" s="9" t="n"/>
       <c r="F122" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G122" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H122" s="9" t="n"/>
       <c r="I122" s="7" t="n">
@@ -4843,10 +4843,10 @@
       </c>
       <c r="K122" s="9" t="n"/>
       <c r="L122" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M122" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N122" s="9" t="n"/>
     </row>
@@ -4867,7 +4867,7 @@
       </c>
       <c r="E123" s="11" t="n"/>
       <c r="F123" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G123" s="10" t="n">
         <v>1</v>
@@ -4881,10 +4881,10 @@
       </c>
       <c r="K123" s="11" t="n"/>
       <c r="L123" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M123" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N123" s="11" t="n"/>
     </row>
@@ -4902,10 +4902,10 @@
         <v>0</v>
       </c>
       <c r="F124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124" t="n">
         <v>18</v>
@@ -4914,10 +4914,10 @@
         <v>18</v>
       </c>
       <c r="L124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -4934,10 +4934,10 @@
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125" t="n">
         <v>18</v>
@@ -4946,10 +4946,10 @@
         <v>18</v>
       </c>
       <c r="L125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -4967,10 +4967,10 @@
       </c>
       <c r="E126" s="9" t="n"/>
       <c r="F126" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G126" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H126" s="9" t="n"/>
       <c r="I126" s="7" t="n">
@@ -4981,7 +4981,7 @@
       </c>
       <c r="K126" s="9" t="n"/>
       <c r="L126" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M126" s="8" t="n">
         <v>1</v>
@@ -5005,10 +5005,10 @@
       </c>
       <c r="E127" s="11" t="n"/>
       <c r="F127" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G127" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H127" s="11" t="n"/>
       <c r="I127" s="6" t="n">
@@ -5019,10 +5019,10 @@
       </c>
       <c r="K127" s="11" t="n"/>
       <c r="L127" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M127" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N127" s="11" t="n"/>
     </row>
@@ -5040,10 +5040,10 @@
         <v>0</v>
       </c>
       <c r="F128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I128" t="n">
         <v>18</v>
@@ -5052,10 +5052,10 @@
         <v>18</v>
       </c>
       <c r="L128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -5072,10 +5072,10 @@
         <v>0</v>
       </c>
       <c r="F129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I129" t="n">
         <v>18</v>
@@ -5084,10 +5084,10 @@
         <v>18</v>
       </c>
       <c r="L129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -5105,10 +5105,10 @@
       </c>
       <c r="E130" s="9" t="n"/>
       <c r="F130" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G130" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H130" s="9" t="n"/>
       <c r="I130" s="7" t="n">
@@ -5143,10 +5143,10 @@
       </c>
       <c r="E131" s="11" t="n"/>
       <c r="F131" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G131" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H131" s="11" t="n"/>
       <c r="I131" s="6" t="n">
@@ -5157,10 +5157,10 @@
       </c>
       <c r="K131" s="11" t="n"/>
       <c r="L131" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M131" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N131" s="11" t="n"/>
     </row>
@@ -5178,10 +5178,10 @@
         <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I132" t="n">
         <v>18</v>
@@ -5190,10 +5190,10 @@
         <v>18</v>
       </c>
       <c r="L132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
@@ -5210,10 +5210,10 @@
         <v>0</v>
       </c>
       <c r="F133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I133" t="n">
         <v>18</v>
@@ -5222,10 +5222,10 @@
         <v>18</v>
       </c>
       <c r="L133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -5243,10 +5243,10 @@
       </c>
       <c r="E134" s="9" t="n"/>
       <c r="F134" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G134" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H134" s="9" t="n"/>
       <c r="I134" s="7" t="n">
@@ -5281,10 +5281,10 @@
       </c>
       <c r="E135" s="11" t="n"/>
       <c r="F135" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G135" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H135" s="11" t="n"/>
       <c r="I135" s="6" t="n">
@@ -5295,10 +5295,10 @@
       </c>
       <c r="K135" s="11" t="n"/>
       <c r="L135" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M135" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N135" s="11" t="n"/>
     </row>
@@ -5316,10 +5316,10 @@
         <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I136" t="n">
         <v>18</v>
@@ -5328,10 +5328,10 @@
         <v>18</v>
       </c>
       <c r="L136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -5348,10 +5348,10 @@
         <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I137" t="n">
         <v>18</v>
@@ -5360,10 +5360,10 @@
         <v>18</v>
       </c>
       <c r="L137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -5381,10 +5381,10 @@
       </c>
       <c r="E138" s="9" t="n"/>
       <c r="F138" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G138" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H138" s="9" t="n"/>
       <c r="I138" s="7" t="n">
@@ -5419,10 +5419,10 @@
       </c>
       <c r="E139" s="11" t="n"/>
       <c r="F139" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G139" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H139" s="11" t="n"/>
       <c r="I139" s="6" t="n">
@@ -5433,10 +5433,10 @@
       </c>
       <c r="K139" s="11" t="n"/>
       <c r="L139" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M139" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N139" s="11" t="n"/>
     </row>
@@ -5454,10 +5454,10 @@
         <v>0</v>
       </c>
       <c r="F140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I140" t="n">
         <v>18</v>
@@ -5466,10 +5466,10 @@
         <v>18</v>
       </c>
       <c r="L140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
@@ -5486,10 +5486,10 @@
         <v>0</v>
       </c>
       <c r="F141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I141" t="n">
         <v>18</v>
@@ -5498,10 +5498,10 @@
         <v>18</v>
       </c>
       <c r="L141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -5519,10 +5519,10 @@
       </c>
       <c r="E142" s="9" t="n"/>
       <c r="F142" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G142" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H142" s="9" t="n"/>
       <c r="I142" s="7" t="n">
@@ -5557,10 +5557,10 @@
       </c>
       <c r="E143" s="11" t="n"/>
       <c r="F143" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G143" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H143" s="11" t="n"/>
       <c r="I143" s="6" t="n">
@@ -5571,10 +5571,10 @@
       </c>
       <c r="K143" s="11" t="n"/>
       <c r="L143" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M143" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N143" s="11" t="n"/>
     </row>
@@ -5592,10 +5592,10 @@
         <v>0</v>
       </c>
       <c r="F144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I144" t="n">
         <v>18</v>
@@ -5604,10 +5604,10 @@
         <v>18</v>
       </c>
       <c r="L144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -5624,10 +5624,10 @@
         <v>0</v>
       </c>
       <c r="F145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I145" t="n">
         <v>18</v>
@@ -5636,10 +5636,10 @@
         <v>18</v>
       </c>
       <c r="L145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -5657,10 +5657,10 @@
       </c>
       <c r="E146" s="9" t="n"/>
       <c r="F146" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G146" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H146" s="9" t="n"/>
       <c r="I146" s="7" t="n">
@@ -5695,10 +5695,10 @@
       </c>
       <c r="E147" s="11" t="n"/>
       <c r="F147" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G147" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H147" s="11" t="n"/>
       <c r="I147" s="6" t="n">
@@ -5709,10 +5709,10 @@
       </c>
       <c r="K147" s="11" t="n"/>
       <c r="L147" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M147" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N147" s="11" t="n"/>
     </row>
@@ -5730,10 +5730,10 @@
         <v>0</v>
       </c>
       <c r="F148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I148" t="n">
         <v>18</v>
@@ -5742,10 +5742,10 @@
         <v>18</v>
       </c>
       <c r="L148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -5762,10 +5762,10 @@
         <v>0</v>
       </c>
       <c r="F149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I149" t="n">
         <v>18</v>
@@ -5774,10 +5774,10 @@
         <v>18</v>
       </c>
       <c r="L149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -5795,10 +5795,10 @@
       </c>
       <c r="E150" s="9" t="n"/>
       <c r="F150" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G150" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H150" s="9" t="n"/>
       <c r="I150" s="7" t="n">
@@ -5833,10 +5833,10 @@
       </c>
       <c r="E151" s="11" t="n"/>
       <c r="F151" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G151" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H151" s="11" t="n"/>
       <c r="I151" s="6" t="n">
@@ -5847,10 +5847,10 @@
       </c>
       <c r="K151" s="11" t="n"/>
       <c r="L151" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M151" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N151" s="11" t="n"/>
     </row>
@@ -5868,10 +5868,10 @@
         <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I152" t="n">
         <v>18</v>
@@ -5880,10 +5880,10 @@
         <v>18</v>
       </c>
       <c r="L152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -5900,10 +5900,10 @@
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I153" t="n">
         <v>18</v>
@@ -5912,10 +5912,10 @@
         <v>18</v>
       </c>
       <c r="L153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -5933,10 +5933,10 @@
       </c>
       <c r="E154" s="9" t="n"/>
       <c r="F154" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G154" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H154" s="9" t="n"/>
       <c r="I154" s="7" t="n">
@@ -5971,10 +5971,10 @@
       </c>
       <c r="E155" s="11" t="n"/>
       <c r="F155" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G155" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H155" s="11" t="n"/>
       <c r="I155" s="6" t="n">
@@ -5985,10 +5985,10 @@
       </c>
       <c r="K155" s="11" t="n"/>
       <c r="L155" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M155" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N155" s="11" t="n"/>
     </row>
@@ -6006,10 +6006,10 @@
         <v>0</v>
       </c>
       <c r="F156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I156" t="n">
         <v>18</v>
@@ -6018,10 +6018,10 @@
         <v>18</v>
       </c>
       <c r="L156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -6038,10 +6038,10 @@
         <v>0</v>
       </c>
       <c r="F157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I157" t="n">
         <v>18</v>
@@ -6050,10 +6050,10 @@
         <v>18</v>
       </c>
       <c r="L157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -6071,10 +6071,10 @@
       </c>
       <c r="E158" s="9" t="n"/>
       <c r="F158" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G158" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H158" s="9" t="n"/>
       <c r="I158" s="7" t="n">
@@ -6109,10 +6109,10 @@
       </c>
       <c r="E159" s="11" t="n"/>
       <c r="F159" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G159" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H159" s="11" t="n"/>
       <c r="I159" s="6" t="n">
@@ -6123,10 +6123,10 @@
       </c>
       <c r="K159" s="11" t="n"/>
       <c r="L159" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M159" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N159" s="11" t="n"/>
     </row>
@@ -6156,10 +6156,10 @@
         <v>18</v>
       </c>
       <c r="L160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -6176,10 +6176,10 @@
         <v>0</v>
       </c>
       <c r="F161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I161" t="n">
         <v>18</v>
@@ -6188,10 +6188,10 @@
         <v>18</v>
       </c>
       <c r="L161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -6209,10 +6209,10 @@
       </c>
       <c r="E162" s="9" t="n"/>
       <c r="F162" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G162" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H162" s="9" t="n"/>
       <c r="I162" s="7" t="n">
@@ -6247,10 +6247,10 @@
       </c>
       <c r="E163" s="11" t="n"/>
       <c r="F163" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G163" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H163" s="11" t="n"/>
       <c r="I163" s="6" t="n">
@@ -6261,10 +6261,10 @@
       </c>
       <c r="K163" s="11" t="n"/>
       <c r="L163" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M163" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N163" s="11" t="n"/>
     </row>
@@ -6282,10 +6282,10 @@
         <v>0</v>
       </c>
       <c r="F164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I164" t="n">
         <v>18</v>
@@ -6294,10 +6294,10 @@
         <v>18</v>
       </c>
       <c r="L164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -6314,10 +6314,10 @@
         <v>0</v>
       </c>
       <c r="F165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I165" t="n">
         <v>18</v>
@@ -6326,10 +6326,10 @@
         <v>18</v>
       </c>
       <c r="L165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1" s="5" thickBot="1">
@@ -6347,10 +6347,10 @@
       </c>
       <c r="E166" s="9" t="n"/>
       <c r="F166" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G166" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H166" s="9" t="n"/>
       <c r="I166" s="7" t="n">

</xml_diff>

<commit_message>
solved bug in indicator
</commit_message>
<xml_diff>
--- a/risk_indicators.xlsx
+++ b/risk_indicators.xlsx
@@ -904,10 +904,10 @@
         <v/>
       </c>
       <c r="W3" s="1" t="n">
-        <v>1.409124149259327</v>
+        <v>1.341918521015387</v>
       </c>
       <c r="X3" t="n">
-        <v>1.412513551050886</v>
+        <v>1.39668576191086</v>
       </c>
       <c r="Y3" s="2">
         <f>(W3-X3)/X3</f>
@@ -990,10 +990,10 @@
         <v/>
       </c>
       <c r="W4" s="1" t="n">
-        <v>1.481490638908731</v>
+        <v>1.471813954999379</v>
       </c>
       <c r="X4" t="n">
-        <v>1.48111166567521</v>
+        <v>1.472900366327911</v>
       </c>
       <c r="Y4" s="2">
         <f>(W4-X4)/X4</f>
@@ -1076,10 +1076,10 @@
         <v/>
       </c>
       <c r="W5" s="1" t="n">
-        <v>1.354639206771643</v>
+        <v>1.365348369177526</v>
       </c>
       <c r="X5" t="n">
-        <v>1.3500922786201</v>
+        <v>1.356252746272316</v>
       </c>
       <c r="Y5" s="2">
         <f>(W5-X5)/X5</f>
@@ -1162,10 +1162,10 @@
         <v/>
       </c>
       <c r="W6" s="5" t="n">
-        <v>0.6240154228978327</v>
+        <v>0.7305066460837168</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>0.6240154228978327</v>
+        <v>0.7462544375031713</v>
       </c>
       <c r="Y6" s="2">
         <f>(W6-X6)/X6</f>
@@ -1239,7 +1239,7 @@
         <v>0.2866379310344828</v>
       </c>
       <c r="T7" s="8" t="n">
-        <v>0.1487068965517242</v>
+        <v>0</v>
       </c>
       <c r="U7" s="8">
         <f>(T7-S7)/S7</f>
@@ -1355,10 +1355,10 @@
         <v>0.6153846153846154</v>
       </c>
       <c r="I9" t="n">
-        <v>0.6153846153846154</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5384615384615384</v>
+        <v>0</v>
       </c>
       <c r="K9" s="8">
         <f>(J9-I9)/I9</f>
@@ -1553,10 +1553,10 @@
         <v>1</v>
       </c>
       <c r="S11" s="4" t="n">
-        <v>1</v>
+        <v>0.9886104783599089</v>
       </c>
       <c r="T11" s="8" t="n">
-        <v>1</v>
+        <v>0.4419134396355353</v>
       </c>
       <c r="U11" s="8">
         <f>(T11-S11)/S11</f>
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="8" t="n">
-        <v>0.6190476190476191</v>
+        <v>0.2519893899204244</v>
       </c>
       <c r="K15" s="8">
         <f>(J15-I15)/I15</f>
@@ -2136,10 +2136,10 @@
         <v>0.4157303370786517</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>0.4606741573033708</v>
+        <v>0.4382022471910112</v>
       </c>
       <c r="J19" s="8" t="n">
-        <v>0.550561797752809</v>
+        <v>0.348314606741573</v>
       </c>
       <c r="K19" s="8">
         <f>(J19-I19)/I19</f>
@@ -4887,13 +4887,13 @@
         <v/>
       </c>
       <c r="H55" s="12" t="n">
-        <v>1</v>
+        <v>0.8503401360544192</v>
       </c>
       <c r="I55" s="4" t="n">
         <v>1</v>
       </c>
       <c r="J55" s="8" t="n">
-        <v>0.6956521739130435</v>
+        <v>0.1533742331288344</v>
       </c>
       <c r="K55" s="8">
         <f>(J55-I55)/I55</f>
@@ -5199,7 +5199,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="8" t="n">
-        <v>0.5934959349593496</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="K59" s="8">
         <f>(J59-I59)/I59</f>
@@ -5499,13 +5499,13 @@
         <v/>
       </c>
       <c r="H63" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" s="8" t="n">
-        <v>0</v>
+        <v>0.06478873239436622</v>
       </c>
       <c r="K63" s="8">
         <f>(J63-I63)/I63</f>
@@ -5805,10 +5805,10 @@
         <v/>
       </c>
       <c r="H67" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" s="4" t="n">
-        <v>0</v>
+        <v>0.6279069767441861</v>
       </c>
       <c r="J67" s="8" t="n">
         <v>0</v>
@@ -6111,13 +6111,13 @@
         <v/>
       </c>
       <c r="H71" s="12" t="n">
-        <v>0.846938775510204</v>
+        <v>0</v>
       </c>
       <c r="I71" s="4" t="n">
-        <v>0.6224489795918368</v>
+        <v>0</v>
       </c>
       <c r="J71" s="8" t="n">
-        <v>0.5612244897959184</v>
+        <v>0</v>
       </c>
       <c r="K71" s="8">
         <f>(J71-I71)/I71</f>
@@ -6417,13 +6417,13 @@
         <v/>
       </c>
       <c r="H75" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J75" s="8" t="n">
-        <v>0.8378378378378378</v>
+        <v>0</v>
       </c>
       <c r="K75" s="8">
         <f>(J75-I75)/I75</f>
@@ -6493,7 +6493,7 @@
         <v/>
       </c>
       <c r="H76" t="n">
-        <v>0</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="I76" t="n">
         <v>0</v>
@@ -6723,13 +6723,13 @@
         <v/>
       </c>
       <c r="H79" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I79" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" s="8" t="n">
-        <v>0</v>
+        <v>0.3895348837209303</v>
       </c>
       <c r="K79" s="8">
         <f>(J79-I79)/I79</f>
@@ -7032,10 +7032,10 @@
         <v>0</v>
       </c>
       <c r="I83" s="4" t="n">
-        <v>0</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="J83" s="8" t="n">
-        <v>0</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="K83" s="8">
         <f>(J83-I83)/I83</f>
@@ -8411,7 +8411,7 @@
         <v>0</v>
       </c>
       <c r="J101" t="n">
-        <v>0</v>
+        <v>0.01785714285714279</v>
       </c>
       <c r="K101" s="8">
         <f>(J101-I101)/I101</f>
@@ -8445,7 +8445,7 @@
         <v>1</v>
       </c>
       <c r="T101" t="n">
-        <v>1</v>
+        <v>0.9821428571428572</v>
       </c>
       <c r="U101" s="8">
         <f>(T101-S101)/S101</f>
@@ -9171,13 +9171,13 @@
         <v/>
       </c>
       <c r="H111" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I111" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111" s="8" t="n">
-        <v>0</v>
+        <v>0.2392156862745098</v>
       </c>
       <c r="K111" s="8">
         <f>(J111-I111)/I111</f>
@@ -9247,13 +9247,13 @@
         <v/>
       </c>
       <c r="H112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J112" t="n">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="K112" s="8">
         <f>(J112-I112)/I112</f>
@@ -9281,7 +9281,7 @@
         <v/>
       </c>
       <c r="R112" t="n">
-        <v>0.950863213811421</v>
+        <v>1</v>
       </c>
       <c r="S112" t="n">
         <v>1</v>
@@ -9326,10 +9326,10 @@
         <v>0</v>
       </c>
       <c r="I113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K113" s="8">
         <f>(J113-I113)/I113</f>
@@ -9477,13 +9477,13 @@
         <v/>
       </c>
       <c r="H115" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I115" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J115" s="8" t="n">
-        <v>0</v>
+        <v>0.1888888888888889</v>
       </c>
       <c r="K115" s="8">
         <f>(J115-I115)/I115</f>
@@ -9553,13 +9553,13 @@
         <v/>
       </c>
       <c r="H116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J116" t="n">
-        <v>0.6097560975609756</v>
+        <v>0</v>
       </c>
       <c r="K116" s="8">
         <f>(J116-I116)/I116</f>
@@ -9587,7 +9587,7 @@
         <v/>
       </c>
       <c r="R116" t="n">
-        <v>0.9747675962815405</v>
+        <v>1</v>
       </c>
       <c r="S116" t="n">
         <v>1</v>
@@ -9783,13 +9783,13 @@
         <v/>
       </c>
       <c r="H119" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I119" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J119" s="8" t="n">
-        <v>0</v>
+        <v>0.3736263736263736</v>
       </c>
       <c r="K119" s="8">
         <f>(J119-I119)/I119</f>
@@ -10092,10 +10092,10 @@
         <v>0</v>
       </c>
       <c r="I123" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J123" s="8" t="n">
-        <v>0</v>
+        <v>0.08571428571428574</v>
       </c>
       <c r="K123" s="8">
         <f>(J123-I123)/I123</f>
@@ -10165,13 +10165,13 @@
         <v/>
       </c>
       <c r="H124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J124" t="n">
-        <v>0.696969696969697</v>
+        <v>0</v>
       </c>
       <c r="K124" s="8">
         <f>(J124-I124)/I124</f>
@@ -10199,13 +10199,13 @@
         <v/>
       </c>
       <c r="R124" t="n">
-        <v>0.9482288828337875</v>
+        <v>1</v>
       </c>
       <c r="S124" t="n">
-        <v>0.9863760217983651</v>
+        <v>1</v>
       </c>
       <c r="T124" t="n">
-        <v>0.9618528610354223</v>
+        <v>1</v>
       </c>
       <c r="U124" s="8">
         <f>(T124-S124)/S124</f>
@@ -10395,13 +10395,13 @@
         <v/>
       </c>
       <c r="H127" s="12" t="n">
-        <v>1</v>
+        <v>0.8579881656804733</v>
       </c>
       <c r="I127" s="4" t="n">
-        <v>1</v>
+        <v>0.8698224852071006</v>
       </c>
       <c r="J127" s="8" t="n">
-        <v>0.6046511627906976</v>
+        <v>0.2280701754385965</v>
       </c>
       <c r="K127" s="8">
         <f>(J127-I127)/I127</f>
@@ -10429,13 +10429,13 @@
         <v/>
       </c>
       <c r="R127" s="12" t="n">
-        <v>0.8172043010752689</v>
+        <v>1</v>
       </c>
       <c r="S127" s="4" t="n">
-        <v>0.7741935483870968</v>
+        <v>1</v>
       </c>
       <c r="T127" s="8" t="n">
-        <v>0.7455197132616488</v>
+        <v>1</v>
       </c>
       <c r="U127" s="8">
         <f>(T127-S127)/S127</f>
@@ -10471,13 +10471,13 @@
         <v/>
       </c>
       <c r="H128" t="n">
-        <v>0.5102040816326531</v>
+        <v>0</v>
       </c>
       <c r="I128" t="n">
-        <v>0.7142857142857143</v>
+        <v>0</v>
       </c>
       <c r="J128" t="n">
-        <v>0.6734693877551021</v>
+        <v>0</v>
       </c>
       <c r="K128" s="8">
         <f>(J128-I128)/I128</f>
@@ -10701,13 +10701,13 @@
         <v/>
       </c>
       <c r="H131" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I131" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J131" s="8" t="n">
-        <v>0.5675675675675675</v>
+        <v>0</v>
       </c>
       <c r="K131" s="8">
         <f>(J131-I131)/I131</f>
@@ -11007,13 +11007,13 @@
         <v/>
       </c>
       <c r="H135" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I135" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J135" s="8" t="n">
-        <v>0</v>
+        <v>0.3518005540166205</v>
       </c>
       <c r="K135" s="8">
         <f>(J135-I135)/I135</f>
@@ -11041,13 +11041,13 @@
         <v/>
       </c>
       <c r="R135" s="12" t="n">
-        <v>1</v>
+        <v>0.8423963133640553</v>
       </c>
       <c r="S135" s="4" t="n">
-        <v>1</v>
+        <v>0.8645161290322581</v>
       </c>
       <c r="T135" s="8" t="n">
-        <v>1</v>
+        <v>0.8866359447004608</v>
       </c>
       <c r="U135" s="8">
         <f>(T135-S135)/S135</f>
@@ -11083,13 +11083,13 @@
         <v/>
       </c>
       <c r="H136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J136" t="n">
-        <v>0</v>
+        <v>0.2752043596730245</v>
       </c>
       <c r="K136" s="8">
         <f>(J136-I136)/I136</f>
@@ -11117,7 +11117,7 @@
         <v/>
       </c>
       <c r="R136" t="n">
-        <v>1</v>
+        <v>0.990990990990991</v>
       </c>
       <c r="S136" t="n">
         <v>1</v>
@@ -11313,13 +11313,13 @@
         <v/>
       </c>
       <c r="H139" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I139" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J139" s="8" t="n">
-        <v>0</v>
+        <v>0.3594771241830066</v>
       </c>
       <c r="K139" s="8">
         <f>(J139-I139)/I139</f>
@@ -11347,13 +11347,13 @@
         <v/>
       </c>
       <c r="R139" s="12" t="n">
-        <v>1</v>
+        <v>0.828169014084507</v>
       </c>
       <c r="S139" s="4" t="n">
-        <v>1</v>
+        <v>0.8262910798122066</v>
       </c>
       <c r="T139" s="8" t="n">
-        <v>1</v>
+        <v>0.8413145539906103</v>
       </c>
       <c r="U139" s="8">
         <f>(T139-S139)/S139</f>
@@ -11389,13 +11389,13 @@
         <v/>
       </c>
       <c r="H140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J140" t="n">
-        <v>0</v>
+        <v>0.3848580441640379</v>
       </c>
       <c r="K140" s="8">
         <f>(J140-I140)/I140</f>
@@ -11423,13 +11423,13 @@
         <v/>
       </c>
       <c r="R140" t="n">
-        <v>1</v>
+        <v>0.7076566125290024</v>
       </c>
       <c r="S140" t="n">
-        <v>1</v>
+        <v>0.777262180974478</v>
       </c>
       <c r="T140" t="n">
-        <v>1</v>
+        <v>0.8097447795823666</v>
       </c>
       <c r="U140" s="8">
         <f>(T140-S140)/S140</f>
@@ -11625,7 +11625,7 @@
         <v>1</v>
       </c>
       <c r="J143" s="8" t="n">
-        <v>1</v>
+        <v>0.3625304136253041</v>
       </c>
       <c r="K143" s="8">
         <f>(J143-I143)/I143</f>
@@ -11653,13 +11653,13 @@
         <v/>
       </c>
       <c r="R143" s="12" t="n">
-        <v>0.8207343412526998</v>
+        <v>0.8291316526610645</v>
       </c>
       <c r="S143" s="4" t="n">
-        <v>0.8509719222462203</v>
+        <v>0.8141923436041083</v>
       </c>
       <c r="T143" s="8" t="n">
-        <v>0.8185745140388769</v>
+        <v>0.830999066293184</v>
       </c>
       <c r="U143" s="8">
         <f>(T143-S143)/S143</f>
@@ -11695,13 +11695,13 @@
         <v/>
       </c>
       <c r="H144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J144" t="n">
-        <v>0</v>
+        <v>0.4036939313984169</v>
       </c>
       <c r="K144" s="8">
         <f>(J144-I144)/I144</f>
@@ -11729,13 +11729,13 @@
         <v/>
       </c>
       <c r="R144" t="n">
-        <v>1</v>
+        <v>0.5868814729574223</v>
       </c>
       <c r="S144" t="n">
-        <v>1</v>
+        <v>0.6536248561565017</v>
       </c>
       <c r="T144" t="n">
-        <v>1</v>
+        <v>0.6881472957422324</v>
       </c>
       <c r="U144" s="8">
         <f>(T144-S144)/S144</f>
@@ -11925,13 +11925,13 @@
         <v/>
       </c>
       <c r="H147" s="12" t="n">
-        <v>0.6835443037974683</v>
+        <v>1</v>
       </c>
       <c r="I147" s="4" t="n">
-        <v>0.4936708860759493</v>
+        <v>1</v>
       </c>
       <c r="J147" s="8" t="n">
-        <v>0.5569620253164558</v>
+        <v>0.3192771084337349</v>
       </c>
       <c r="K147" s="8">
         <f>(J147-I147)/I147</f>
@@ -11962,10 +11962,10 @@
         <v>1</v>
       </c>
       <c r="S147" s="4" t="n">
-        <v>1</v>
+        <v>0.9663941871026339</v>
       </c>
       <c r="T147" s="8" t="n">
-        <v>1</v>
+        <v>0.9809264305177112</v>
       </c>
       <c r="U147" s="8">
         <f>(T147-S147)/S147</f>
@@ -12001,13 +12001,13 @@
         <v/>
       </c>
       <c r="H148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J148" t="n">
-        <v>0</v>
+        <v>0.4399999999999999</v>
       </c>
       <c r="K148" s="8">
         <f>(J148-I148)/I148</f>
@@ -12035,13 +12035,13 @@
         <v/>
       </c>
       <c r="R148" t="n">
-        <v>1</v>
+        <v>0.7206385404789054</v>
       </c>
       <c r="S148" t="n">
-        <v>1</v>
+        <v>0.8164196123147093</v>
       </c>
       <c r="T148" t="n">
-        <v>1</v>
+        <v>0.8415051311288484</v>
       </c>
       <c r="U148" s="8">
         <f>(T148-S148)/S148</f>
@@ -12231,13 +12231,13 @@
         <v/>
       </c>
       <c r="H151" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I151" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J151" s="8" t="n">
-        <v>0</v>
+        <v>0.4167371090448013</v>
       </c>
       <c r="K151" s="8">
         <f>(J151-I151)/I151</f>
@@ -12265,13 +12265,13 @@
         <v/>
       </c>
       <c r="R151" s="12" t="n">
-        <v>1</v>
+        <v>0.7049873203719358</v>
       </c>
       <c r="S151" s="4" t="n">
-        <v>1</v>
+        <v>0.5562130177514792</v>
       </c>
       <c r="T151" s="8" t="n">
-        <v>1</v>
+        <v>0.5832628909551987</v>
       </c>
       <c r="U151" s="8">
         <f>(T151-S151)/S151</f>
@@ -12307,13 +12307,13 @@
         <v/>
       </c>
       <c r="H152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J152" t="n">
-        <v>0</v>
+        <v>0.4449152542372882</v>
       </c>
       <c r="K152" s="8">
         <f>(J152-I152)/I152</f>
@@ -12341,13 +12341,13 @@
         <v/>
       </c>
       <c r="R152" t="n">
-        <v>1</v>
+        <v>0.8715415019762845</v>
       </c>
       <c r="S152" t="n">
-        <v>1</v>
+        <v>0.9387351778656127</v>
       </c>
       <c r="T152" t="n">
-        <v>1</v>
+        <v>0.9624505928853755</v>
       </c>
       <c r="U152" s="8">
         <f>(T152-S152)/S152</f>
@@ -12537,13 +12537,13 @@
         <v/>
       </c>
       <c r="H155" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I155" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J155" s="8" t="n">
-        <v>0</v>
+        <v>0.6833333333333333</v>
       </c>
       <c r="K155" s="8">
         <f>(J155-I155)/I155</f>
@@ -12571,13 +12571,13 @@
         <v/>
       </c>
       <c r="R155" s="12" t="n">
-        <v>1</v>
+        <v>0.4433333333333334</v>
       </c>
       <c r="S155" s="4" t="n">
-        <v>1</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="T155" s="8" t="n">
-        <v>1</v>
+        <v>0.3166666666666667</v>
       </c>
       <c r="U155" s="8">
         <f>(T155-S155)/S155</f>
@@ -12613,13 +12613,13 @@
         <v/>
       </c>
       <c r="H156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J156" t="n">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="K156" s="8">
         <f>(J156-I156)/I156</f>
@@ -12843,13 +12843,13 @@
         <v/>
       </c>
       <c r="H159" s="12" t="n">
-        <v>0.2261904761904762</v>
+        <v>1</v>
       </c>
       <c r="I159" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J159" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K159" s="8">
         <f>(J159-I159)/I159</f>
@@ -12877,13 +12877,13 @@
         <v/>
       </c>
       <c r="R159" s="12" t="n">
-        <v>1</v>
+        <v>0.006546644844517169</v>
       </c>
       <c r="S159" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T159" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U159" s="8">
         <f>(T159-S159)/S159</f>
@@ -12919,13 +12919,13 @@
         <v/>
       </c>
       <c r="H160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J160" t="n">
-        <v>0</v>
+        <v>0.8297872340425532</v>
       </c>
       <c r="K160" s="8">
         <f>(J160-I160)/I160</f>
@@ -12953,13 +12953,13 @@
         <v/>
       </c>
       <c r="R160" t="n">
-        <v>1</v>
+        <v>0.1814814814814815</v>
       </c>
       <c r="S160" t="n">
-        <v>1</v>
+        <v>0.1518518518518519</v>
       </c>
       <c r="T160" t="n">
-        <v>1</v>
+        <v>0.1851851851851851</v>
       </c>
       <c r="U160" s="8">
         <f>(T160-S160)/S160</f>
@@ -12995,13 +12995,13 @@
         <v/>
       </c>
       <c r="H161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K161" s="8">
         <f>(J161-I161)/I161</f>
@@ -13029,13 +13029,13 @@
         <v/>
       </c>
       <c r="R161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U161" s="8">
         <f>(T161-S161)/S161</f>
@@ -13149,13 +13149,13 @@
         <v/>
       </c>
       <c r="H163" s="12" t="n">
-        <v>0.1603053435114504</v>
+        <v>1</v>
       </c>
       <c r="I163" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J163" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K163" s="8">
         <f>(J163-I163)/I163</f>
@@ -13183,13 +13183,13 @@
         <v/>
       </c>
       <c r="R163" s="12" t="n">
-        <v>1</v>
+        <v>0.2074829931972789</v>
       </c>
       <c r="S163" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T163" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U163" s="8">
         <f>(T163-S163)/S163</f>
@@ -13225,13 +13225,13 @@
         <v/>
       </c>
       <c r="H164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J164" t="n">
-        <v>0</v>
+        <v>0.9318181818181818</v>
       </c>
       <c r="K164" s="8">
         <f>(J164-I164)/I164</f>
@@ -13259,13 +13259,13 @@
         <v/>
       </c>
       <c r="R164" t="n">
-        <v>1</v>
+        <v>0.4295302013422819</v>
       </c>
       <c r="S164" t="n">
-        <v>1</v>
+        <v>0.3911792905081496</v>
       </c>
       <c r="T164" t="n">
-        <v>1</v>
+        <v>0.4218600191754553</v>
       </c>
       <c r="U164" s="8">
         <f>(T164-S164)/S164</f>
@@ -13301,13 +13301,13 @@
         <v/>
       </c>
       <c r="H165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J165" t="n">
-        <v>0</v>
+        <v>0.5114503816793894</v>
       </c>
       <c r="K165" s="8">
         <f>(J165-I165)/I165</f>
@@ -13335,13 +13335,13 @@
         <v/>
       </c>
       <c r="R165" t="n">
-        <v>1</v>
+        <v>0.366412213740458</v>
       </c>
       <c r="S165" t="n">
-        <v>1</v>
+        <v>0.366412213740458</v>
       </c>
       <c r="T165" t="n">
-        <v>1</v>
+        <v>0.4885496183206106</v>
       </c>
       <c r="U165" s="8">
         <f>(T165-S165)/S165</f>

</xml_diff>

<commit_message>
show D and R distribution
</commit_message>
<xml_diff>
--- a/risk_indicators.xlsx
+++ b/risk_indicators.xlsx
@@ -904,10 +904,10 @@
         <v/>
       </c>
       <c r="W3" s="1" t="n">
-        <v>1.147331546857365</v>
+        <v>0.9908069294577841</v>
       </c>
       <c r="X3" t="n">
-        <v>1.263490971854047</v>
+        <v>1.176114895843392</v>
       </c>
       <c r="Y3" s="2">
         <f>(W3-X3)/X3</f>
@@ -990,10 +990,10 @@
         <v/>
       </c>
       <c r="W4" s="1" t="n">
-        <v>1.078822186879199</v>
+        <v>0.9215770436919087</v>
       </c>
       <c r="X4" t="n">
-        <v>1.205901382928495</v>
+        <v>1.109184290028507</v>
       </c>
       <c r="Y4" s="2">
         <f>(W4-X4)/X4</f>
@@ -1076,10 +1076,10 @@
         <v/>
       </c>
       <c r="W5" s="1" t="n">
-        <v>0.9392442546712261</v>
+        <v>1.010797866848767</v>
       </c>
       <c r="X5" t="n">
-        <v>1.103020550517574</v>
+        <v>1.242272418015155</v>
       </c>
       <c r="Y5" s="2">
         <f>(W5-X5)/X5</f>
@@ -1162,10 +1162,10 @@
         <v/>
       </c>
       <c r="W6" s="5" t="n">
-        <v>0.7029330991065131</v>
+        <v>0.6464465152908782</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>0.7141775046275405</v>
+        <v>0.6670768192115565</v>
       </c>
       <c r="Y6" s="2">
         <f>(W6-X6)/X6</f>
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="8" t="n">
-        <v>0.7360637087599544</v>
+        <v>0.7298524404086266</v>
       </c>
       <c r="K15" s="8">
         <f>(J15-I15)/I15</f>
@@ -1861,13 +1861,13 @@
         <v/>
       </c>
       <c r="R15" s="12" t="n">
-        <v>0.229806598407281</v>
+        <v>0.2338251986379114</v>
       </c>
       <c r="S15" s="4" t="n">
-        <v>0.229806598407281</v>
+        <v>0.2338251986379114</v>
       </c>
       <c r="T15" s="8" t="n">
-        <v>0.2639362912400456</v>
+        <v>0.2701475595913734</v>
       </c>
       <c r="U15" s="8">
         <f>(T15-S15)/S15</f>
@@ -2139,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="8" t="n">
-        <v>0.5357873210633947</v>
+        <v>0.5788336933045357</v>
       </c>
       <c r="K19" s="8">
         <f>(J19-I19)/I19</f>
@@ -2167,13 +2167,13 @@
         <v/>
       </c>
       <c r="R19" s="12" t="n">
-        <v>0.4314928425357873</v>
+        <v>0.3844492440604752</v>
       </c>
       <c r="S19" s="4" t="n">
-        <v>0.4335378323108384</v>
+        <v>0.386609071274298</v>
       </c>
       <c r="T19" s="8" t="n">
-        <v>0.4642126789366053</v>
+        <v>0.4211663066954643</v>
       </c>
       <c r="U19" s="8">
         <f>(T19-S19)/S19</f>
@@ -2215,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>0.8573281452658885</v>
+        <v>0.9308437067773168</v>
       </c>
       <c r="K20" s="8">
         <f>(J20-I20)/I20</f>
@@ -2243,13 +2243,13 @@
         <v/>
       </c>
       <c r="R20" t="n">
-        <v>0.1037613488975356</v>
+        <v>0.02766251728907332</v>
       </c>
       <c r="S20" t="n">
-        <v>0.1037613488975356</v>
+        <v>0.02766251728907332</v>
       </c>
       <c r="T20" t="n">
-        <v>0.1426718547341115</v>
+        <v>0.06915629322268324</v>
       </c>
       <c r="U20" s="8">
         <f>(T20-S20)/S20</f>
@@ -2445,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="8" t="n">
-        <v>0.6222023276633841</v>
+        <v>0.7497435897435898</v>
       </c>
       <c r="K23" s="8">
         <f>(J23-I23)/I23</f>
@@ -2473,13 +2473,13 @@
         <v/>
       </c>
       <c r="R23" s="12" t="n">
-        <v>0.2059086839749329</v>
+        <v>0.05128205128205132</v>
       </c>
       <c r="S23" s="4" t="n">
-        <v>0.350940017905103</v>
+        <v>0.2174358974358974</v>
       </c>
       <c r="T23" s="8" t="n">
-        <v>0.3777976723366159</v>
+        <v>0.2502564102564102</v>
       </c>
       <c r="U23" s="8">
         <f>(T23-S23)/S23</f>
@@ -2521,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>0.4905450500556173</v>
+        <v>0.629242819843342</v>
       </c>
       <c r="K24" s="8">
         <f>(J24-I24)/I24</f>
@@ -2549,13 +2549,13 @@
         <v/>
       </c>
       <c r="R24" t="n">
-        <v>0.4783092324805339</v>
+        <v>0.3394255874673628</v>
       </c>
       <c r="S24" t="n">
-        <v>0.4805339265850945</v>
+        <v>0.3420365535248042</v>
       </c>
       <c r="T24" t="n">
-        <v>0.5094549499443827</v>
+        <v>0.370757180156658</v>
       </c>
       <c r="U24" s="8">
         <f>(T24-S24)/S24</f>
@@ -2779,7 +2779,7 @@
         <v/>
       </c>
       <c r="R27" s="12" t="n">
-        <v>1</v>
+        <v>0.971201588877855</v>
       </c>
       <c r="S27" s="4" t="n">
         <v>1</v>
@@ -2827,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="n">
-        <v>0.4235807860262009</v>
+        <v>0.4279475982532751</v>
       </c>
       <c r="K28" s="8">
         <f>(J28-I28)/I28</f>
@@ -2855,13 +2855,13 @@
         <v/>
       </c>
       <c r="R28" t="n">
-        <v>0.9271948608137045</v>
+        <v>0.9108695652173913</v>
       </c>
       <c r="S28" t="n">
-        <v>0.9293361884368309</v>
+        <v>0.9130434782608695</v>
       </c>
       <c r="T28" t="n">
-        <v>0.9593147751605996</v>
+        <v>0.941304347826087</v>
       </c>
       <c r="U28" s="8">
         <f>(T28-S28)/S28</f>
@@ -3057,7 +3057,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="8" t="n">
-        <v>0.6133209990749307</v>
+        <v>0.8260869565217391</v>
       </c>
       <c r="K31" s="8">
         <f>(J31-I31)/I31</f>
@@ -3085,13 +3085,13 @@
         <v/>
       </c>
       <c r="R31" s="12" t="n">
-        <v>0.3385753931544866</v>
+        <v>0.1181716833890747</v>
       </c>
       <c r="S31" s="4" t="n">
-        <v>0.366327474560592</v>
+        <v>0.1516164994425864</v>
       </c>
       <c r="T31" s="8" t="n">
-        <v>0.3866790009250693</v>
+        <v>0.1739130434782609</v>
       </c>
       <c r="U31" s="8">
         <f>(T31-S31)/S31</f>
@@ -3363,7 +3363,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="8" t="n">
-        <v>0.4098972922502334</v>
+        <v>0.5282817502668089</v>
       </c>
       <c r="K35" s="8">
         <f>(J35-I35)/I35</f>
@@ -3391,13 +3391,13 @@
         <v/>
       </c>
       <c r="R35" s="12" t="n">
-        <v>0.5303454715219421</v>
+        <v>0.4140875133404482</v>
       </c>
       <c r="S35" s="4" t="n">
-        <v>0.5564892623716153</v>
+        <v>0.4439701173959445</v>
       </c>
       <c r="T35" s="8" t="n">
-        <v>0.5901027077497666</v>
+        <v>0.4717182497331911</v>
       </c>
       <c r="U35" s="8">
         <f>(T35-S35)/S35</f>
@@ -3697,13 +3697,13 @@
         <v/>
       </c>
       <c r="R39" s="12" t="n">
-        <v>0.1031746031746031</v>
+        <v>0.0628166160081054</v>
       </c>
       <c r="S39" s="4" t="n">
-        <v>0.07341269841269837</v>
+        <v>0.03242147922998984</v>
       </c>
       <c r="T39" s="8" t="n">
-        <v>0.1051587301587301</v>
+        <v>0.0628166160081054</v>
       </c>
       <c r="U39" s="8">
         <f>(T39-S39)/S39</f>
@@ -4003,13 +4003,13 @@
         <v/>
       </c>
       <c r="R43" s="12" t="n">
-        <v>0.6897689768976898</v>
+        <v>0.5542406311637081</v>
       </c>
       <c r="S43" s="4" t="n">
-        <v>0.740924092409241</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="T43" s="8" t="n">
-        <v>0.764026402640264</v>
+        <v>0.6390532544378699</v>
       </c>
       <c r="U43" s="8">
         <f>(T43-S43)/S43</f>
@@ -4155,13 +4155,13 @@
         <v/>
       </c>
       <c r="R45" t="n">
-        <v>0.6612903225806451</v>
+        <v>0.3383084577114428</v>
       </c>
       <c r="S45" t="n">
-        <v>0.6532258064516129</v>
+        <v>0.3283582089552239</v>
       </c>
       <c r="T45" t="n">
-        <v>0.7903225806451613</v>
+        <v>0.4975124378109452</v>
       </c>
       <c r="U45" s="8">
         <f>(T45-S45)/S45</f>
@@ -4309,13 +4309,13 @@
         <v/>
       </c>
       <c r="R47" s="12" t="n">
-        <v>0.6286161063330727</v>
+        <v>0.515828677839851</v>
       </c>
       <c r="S47" s="4" t="n">
-        <v>0.653635652853792</v>
+        <v>0.5456238361266295</v>
       </c>
       <c r="T47" s="8" t="n">
-        <v>0.6724003127443315</v>
+        <v>0.5716945996275605</v>
       </c>
       <c r="U47" s="8">
         <f>(T47-S47)/S47</f>
@@ -4357,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="J48" t="n">
-        <v>0.4523809523809524</v>
+        <v>0.2781740370898717</v>
       </c>
       <c r="K48" s="8">
         <f>(J48-I48)/I48</f>
@@ -4385,13 +4385,13 @@
         <v/>
       </c>
       <c r="R48" t="n">
-        <v>0.7105263157894737</v>
+        <v>0.8562628336755647</v>
       </c>
       <c r="S48" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.864476386036961</v>
       </c>
       <c r="T48" t="n">
-        <v>0.7424812030075187</v>
+        <v>0.8993839835728953</v>
       </c>
       <c r="U48" s="8">
         <f>(T48-S48)/S48</f>
@@ -4433,7 +4433,7 @@
         <v>1</v>
       </c>
       <c r="J49" t="n">
-        <v>0.1414634146341464</v>
+        <v>0.2513368983957219</v>
       </c>
       <c r="K49" s="8">
         <f>(J49-I49)/I49</f>
@@ -4461,13 +4461,13 @@
         <v/>
       </c>
       <c r="R49" t="n">
-        <v>0.8914728682170543</v>
+        <v>0.5742574257425742</v>
       </c>
       <c r="S49" t="n">
-        <v>0.9689922480620154</v>
+        <v>0.6732673267326733</v>
       </c>
       <c r="T49" t="n">
-        <v>1</v>
+        <v>0.8514851485148515</v>
       </c>
       <c r="U49" s="8">
         <f>(T49-S49)/S49</f>
@@ -4587,7 +4587,7 @@
         <v>1</v>
       </c>
       <c r="J51" s="8" t="n">
-        <v>0.8581081081081081</v>
+        <v>0.9130434782608696</v>
       </c>
       <c r="K51" s="8">
         <f>(J51-I51)/I51</f>
@@ -4615,13 +4615,13 @@
         <v/>
       </c>
       <c r="R51" s="12" t="n">
-        <v>0.4125874125874126</v>
+        <v>0.3767572633552014</v>
       </c>
       <c r="S51" s="4" t="n">
-        <v>0.4458041958041958</v>
+        <v>0.4123711340206185</v>
       </c>
       <c r="T51" s="8" t="n">
-        <v>0.4755244755244755</v>
+        <v>0.4404873477038426</v>
       </c>
       <c r="U51" s="8">
         <f>(T51-S51)/S51</f>
@@ -4663,7 +4663,7 @@
         <v>1</v>
       </c>
       <c r="J52" t="n">
-        <v>0.5432098765432098</v>
+        <v>0.3082489146164978</v>
       </c>
       <c r="K52" s="8">
         <f>(J52-I52)/I52</f>
@@ -4691,13 +4691,13 @@
         <v/>
       </c>
       <c r="R52" t="n">
-        <v>0.6135629709364908</v>
+        <v>0.8294736842105264</v>
       </c>
       <c r="S52" t="n">
-        <v>0.6221743810548978</v>
+        <v>0.84</v>
       </c>
       <c r="T52" t="n">
-        <v>0.6544671689989235</v>
+        <v>0.871578947368421</v>
       </c>
       <c r="U52" s="8">
         <f>(T52-S52)/S52</f>
@@ -4739,7 +4739,7 @@
         <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>0.2839506172839507</v>
+        <v>0.5265700483091788</v>
       </c>
       <c r="K53" s="8">
         <f>(J53-I53)/I53</f>
@@ -4767,13 +4767,13 @@
         <v/>
       </c>
       <c r="R53" t="n">
-        <v>0.4855967078189301</v>
+        <v>0.2028985507246377</v>
       </c>
       <c r="S53" t="n">
-        <v>0.5679012345679012</v>
+        <v>0.2995169082125604</v>
       </c>
       <c r="T53" t="n">
-        <v>0.7160493827160493</v>
+        <v>0.4734299516908212</v>
       </c>
       <c r="U53" s="8">
         <f>(T53-S53)/S53</f>
@@ -4893,7 +4893,7 @@
         <v>1</v>
       </c>
       <c r="J55" s="8" t="n">
-        <v>1</v>
+        <v>0.8990990990990991</v>
       </c>
       <c r="K55" s="8">
         <f>(J55-I55)/I55</f>
@@ -4921,13 +4921,13 @@
         <v/>
       </c>
       <c r="R55" s="12" t="n">
-        <v>0</v>
+        <v>0.05585585585585584</v>
       </c>
       <c r="S55" s="4" t="n">
-        <v>0</v>
+        <v>0.07747747747747746</v>
       </c>
       <c r="T55" s="8" t="n">
-        <v>0</v>
+        <v>0.1009009009009009</v>
       </c>
       <c r="U55" s="8">
         <f>(T55-S55)/S55</f>
@@ -4969,7 +4969,7 @@
         <v>1</v>
       </c>
       <c r="J56" t="n">
-        <v>0.5189873417721519</v>
+        <v>1</v>
       </c>
       <c r="K56" s="8">
         <f>(J56-I56)/I56</f>
@@ -4997,13 +4997,13 @@
         <v/>
       </c>
       <c r="R56" t="n">
-        <v>0.4794188861985472</v>
+        <v>0.300990099009901</v>
       </c>
       <c r="S56" t="n">
-        <v>0.4818401937046004</v>
+        <v>0.304950495049505</v>
       </c>
       <c r="T56" t="n">
-        <v>0.5205811138014528</v>
+        <v>0.3366336633663367</v>
       </c>
       <c r="U56" s="8">
         <f>(T56-S56)/S56</f>
@@ -5275,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>0.8051948051948052</v>
       </c>
       <c r="K60" s="8">
         <f>(J60-I60)/I60</f>
@@ -5303,13 +5303,13 @@
         <v/>
       </c>
       <c r="R60" t="n">
-        <v>0</v>
+        <v>0.1809851088201604</v>
       </c>
       <c r="S60" t="n">
-        <v>0</v>
+        <v>0.1855670103092784</v>
       </c>
       <c r="T60" t="n">
-        <v>0</v>
+        <v>0.2268041237113402</v>
       </c>
       <c r="U60" s="8">
         <f>(T60-S60)/S60</f>
@@ -5733,7 +5733,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="6" t="n">
-        <v>1</v>
+        <v>0.3827160493827161</v>
       </c>
       <c r="K66" s="8">
         <f>(J66-I66)/I66</f>
@@ -5761,13 +5761,13 @@
         <v/>
       </c>
       <c r="R66" s="14" t="n">
-        <v>0</v>
+        <v>0.09876543209876543</v>
       </c>
       <c r="S66" s="5" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="T66" s="6" t="n">
-        <v>0</v>
+        <v>0.6172839506172839</v>
       </c>
       <c r="U66" s="8">
         <f>(T66-S66)/S66</f>
@@ -6033,10 +6033,10 @@
         <v/>
       </c>
       <c r="H70" s="14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J70" s="6" t="n">
         <v>0</v>
@@ -6067,10 +6067,10 @@
         <v/>
       </c>
       <c r="R70" s="14" t="n">
-        <v>0.4347826086956521</v>
+        <v>1</v>
       </c>
       <c r="S70" s="5" t="n">
-        <v>0.927536231884058</v>
+        <v>1</v>
       </c>
       <c r="T70" s="6" t="n">
         <v>1</v>
@@ -6210,7 +6210,7 @@
         <v>1</v>
       </c>
       <c r="O72" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="P72" s="8">
         <f>(O72-N72)/N72</f>
@@ -8787,13 +8787,13 @@
         <v/>
       </c>
       <c r="H106" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I106" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J106" s="6" t="n">
-        <v>0</v>
+        <v>0.03296703296703296</v>
       </c>
       <c r="K106" s="8">
         <f>(J106-I106)/I106</f>
@@ -8821,13 +8821,13 @@
         <v/>
       </c>
       <c r="R106" s="14" t="n">
-        <v>1</v>
+        <v>0.5054945054945055</v>
       </c>
       <c r="S106" s="5" t="n">
-        <v>1</v>
+        <v>0.5934065934065934</v>
       </c>
       <c r="T106" s="6" t="n">
-        <v>1</v>
+        <v>0.967032967032967</v>
       </c>
       <c r="U106" s="8">
         <f>(T106-S106)/S106</f>
@@ -8899,7 +8899,7 @@
         <v/>
       </c>
       <c r="R107" s="12" t="n">
-        <v>0.266857962697274</v>
+        <v>0</v>
       </c>
       <c r="S107" s="4" t="n">
         <v>0</v>
@@ -8975,10 +8975,10 @@
         <v/>
       </c>
       <c r="R108" t="n">
-        <v>0.02635914332784184</v>
+        <v>0</v>
       </c>
       <c r="S108" t="n">
-        <v>0.2273476112026359</v>
+        <v>0</v>
       </c>
       <c r="T108" t="n">
         <v>0</v>
@@ -9096,7 +9096,7 @@
         <v>0</v>
       </c>
       <c r="I110" s="5" t="n">
-        <v>0</v>
+        <v>0.8571428571428572</v>
       </c>
       <c r="J110" s="6" t="n">
         <v>0</v>
@@ -9205,10 +9205,10 @@
         <v/>
       </c>
       <c r="R111" s="12" t="n">
-        <v>0.6057142857142858</v>
+        <v>0</v>
       </c>
       <c r="S111" s="4" t="n">
-        <v>0.1971428571428572</v>
+        <v>0</v>
       </c>
       <c r="T111" s="8" t="n">
         <v>0</v>
@@ -9281,13 +9281,13 @@
         <v/>
       </c>
       <c r="R112" t="n">
-        <v>0.5054945054945055</v>
+        <v>0</v>
       </c>
       <c r="S112" t="n">
-        <v>0.7032967032967034</v>
+        <v>0</v>
       </c>
       <c r="T112" t="n">
-        <v>0.4960753532182103</v>
+        <v>0</v>
       </c>
       <c r="U112" s="8">
         <f>(T112-S112)/S112</f>
@@ -9329,7 +9329,7 @@
         <v>1</v>
       </c>
       <c r="J113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K113" s="8">
         <f>(J113-I113)/I113</f>
@@ -9357,13 +9357,13 @@
         <v/>
       </c>
       <c r="R113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U113" s="8">
         <f>(T113-S113)/S113</f>
@@ -9511,13 +9511,13 @@
         <v/>
       </c>
       <c r="R115" s="12" t="n">
-        <v>0.9596774193548387</v>
+        <v>0</v>
       </c>
       <c r="S115" s="4" t="n">
-        <v>0.7956989247311828</v>
+        <v>0</v>
       </c>
       <c r="T115" s="8" t="n">
-        <v>0.8306451612903226</v>
+        <v>0</v>
       </c>
       <c r="U115" s="8">
         <f>(T115-S115)/S115</f>
@@ -9553,13 +9553,13 @@
         <v/>
       </c>
       <c r="H116" t="n">
-        <v>0.9294117647058824</v>
+        <v>1</v>
       </c>
       <c r="I116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K116" s="8">
         <f>(J116-I116)/I116</f>
@@ -9587,13 +9587,13 @@
         <v/>
       </c>
       <c r="R116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U116" s="8">
         <f>(T116-S116)/S116</f>
@@ -9629,13 +9629,13 @@
         <v/>
       </c>
       <c r="H117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K117" s="8">
         <f>(J117-I117)/I117</f>
@@ -9652,7 +9652,7 @@
         <v>1</v>
       </c>
       <c r="O117" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="P117" s="8">
         <f>(O117-N117)/N117</f>
@@ -9663,13 +9663,13 @@
         <v/>
       </c>
       <c r="R117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U117" s="8">
         <f>(T117-S117)/S117</f>
@@ -9789,7 +9789,7 @@
         <v>1</v>
       </c>
       <c r="J119" s="8" t="n">
-        <v>0.3569739952718676</v>
+        <v>1</v>
       </c>
       <c r="K119" s="8">
         <f>(J119-I119)/I119</f>
@@ -9817,13 +9817,13 @@
         <v/>
       </c>
       <c r="R119" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S119" s="4" t="n">
-        <v>0.9674185463659147</v>
+        <v>0</v>
       </c>
       <c r="T119" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U119" s="8">
         <f>(T119-S119)/S119</f>
@@ -9859,13 +9859,13 @@
         <v/>
       </c>
       <c r="H120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K120" s="8">
         <f>(J120-I120)/I120</f>
@@ -9893,13 +9893,13 @@
         <v/>
       </c>
       <c r="R120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U120" s="8">
         <f>(T120-S120)/S120</f>
@@ -9935,13 +9935,13 @@
         <v/>
       </c>
       <c r="H121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K121" s="8">
         <f>(J121-I121)/I121</f>
@@ -9969,13 +9969,13 @@
         <v/>
       </c>
       <c r="R121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U121" s="8">
         <f>(T121-S121)/S121</f>
@@ -10089,13 +10089,13 @@
         <v/>
       </c>
       <c r="H123" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I123" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J123" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K123" s="8">
         <f>(J123-I123)/I123</f>
@@ -10123,13 +10123,13 @@
         <v/>
       </c>
       <c r="R123" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S123" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T123" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U123" s="8">
         <f>(T123-S123)/S123</f>
@@ -10165,13 +10165,13 @@
         <v/>
       </c>
       <c r="H124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K124" s="8">
         <f>(J124-I124)/I124</f>
@@ -10199,13 +10199,13 @@
         <v/>
       </c>
       <c r="R124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U124" s="8">
         <f>(T124-S124)/S124</f>
@@ -10241,13 +10241,13 @@
         <v/>
       </c>
       <c r="H125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K125" s="8">
         <f>(J125-I125)/I125</f>
@@ -10275,13 +10275,13 @@
         <v/>
       </c>
       <c r="R125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U125" s="8">
         <f>(T125-S125)/S125</f>
@@ -10429,13 +10429,13 @@
         <v/>
       </c>
       <c r="R127" s="12" t="n">
-        <v>0.4285714285714286</v>
+        <v>0</v>
       </c>
       <c r="S127" s="4" t="n">
-        <v>0.4666666666666667</v>
+        <v>0</v>
       </c>
       <c r="T127" s="8" t="n">
-        <v>0.4952380952380953</v>
+        <v>0</v>
       </c>
       <c r="U127" s="8">
         <f>(T127-S127)/S127</f>
@@ -10471,13 +10471,13 @@
         <v/>
       </c>
       <c r="H128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K128" s="8">
         <f>(J128-I128)/I128</f>
@@ -10505,13 +10505,13 @@
         <v/>
       </c>
       <c r="R128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U128" s="8">
         <f>(T128-S128)/S128</f>
@@ -10547,13 +10547,13 @@
         <v/>
       </c>
       <c r="H129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K129" s="8">
         <f>(J129-I129)/I129</f>
@@ -10581,13 +10581,13 @@
         <v/>
       </c>
       <c r="R129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U129" s="8">
         <f>(T129-S129)/S129</f>
@@ -10623,10 +10623,10 @@
         <v/>
       </c>
       <c r="H130" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I130" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J130" s="6" t="n">
         <v>0</v>
@@ -10735,13 +10735,13 @@
         <v/>
       </c>
       <c r="R131" s="12" t="n">
-        <v>0.3516908212560386</v>
+        <v>0</v>
       </c>
       <c r="S131" s="4" t="n">
-        <v>0.3053140096618358</v>
+        <v>0</v>
       </c>
       <c r="T131" s="8" t="n">
-        <v>0.1120772946859904</v>
+        <v>0</v>
       </c>
       <c r="U131" s="8">
         <f>(T131-S131)/S131</f>
@@ -10777,13 +10777,13 @@
         <v/>
       </c>
       <c r="H132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K132" s="8">
         <f>(J132-I132)/I132</f>
@@ -10811,13 +10811,13 @@
         <v/>
       </c>
       <c r="R132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U132" s="8">
         <f>(T132-S132)/S132</f>
@@ -10853,13 +10853,13 @@
         <v/>
       </c>
       <c r="H133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K133" s="8">
         <f>(J133-I133)/I133</f>
@@ -10887,13 +10887,13 @@
         <v/>
       </c>
       <c r="R133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U133" s="8">
         <f>(T133-S133)/S133</f>
@@ -11041,13 +11041,13 @@
         <v/>
       </c>
       <c r="R135" s="12" t="n">
-        <v>0.1947565543071161</v>
+        <v>0</v>
       </c>
       <c r="S135" s="4" t="n">
-        <v>0.2097378277153559</v>
+        <v>0</v>
       </c>
       <c r="T135" s="8" t="n">
-        <v>0.2340823970037453</v>
+        <v>0</v>
       </c>
       <c r="U135" s="8">
         <f>(T135-S135)/S135</f>
@@ -11083,7 +11083,7 @@
         <v/>
       </c>
       <c r="H136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I136" t="n">
         <v>1</v>
@@ -11117,13 +11117,13 @@
         <v/>
       </c>
       <c r="R136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U136" s="8">
         <f>(T136-S136)/S136</f>
@@ -11159,13 +11159,13 @@
         <v/>
       </c>
       <c r="H137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K137" s="8">
         <f>(J137-I137)/I137</f>
@@ -11193,13 +11193,13 @@
         <v/>
       </c>
       <c r="R137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U137" s="8">
         <f>(T137-S137)/S137</f>
@@ -11238,7 +11238,7 @@
         <v>0</v>
       </c>
       <c r="I138" s="5" t="n">
-        <v>0</v>
+        <v>0.05263157894736847</v>
       </c>
       <c r="J138" s="6" t="n">
         <v>0</v>
@@ -11347,13 +11347,13 @@
         <v/>
       </c>
       <c r="R139" s="12" t="n">
-        <v>0.3046875</v>
+        <v>0</v>
       </c>
       <c r="S139" s="4" t="n">
-        <v>0.443359375</v>
+        <v>0</v>
       </c>
       <c r="T139" s="8" t="n">
-        <v>0.474609375</v>
+        <v>0</v>
       </c>
       <c r="U139" s="8">
         <f>(T139-S139)/S139</f>
@@ -11423,13 +11423,13 @@
         <v/>
       </c>
       <c r="R140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T140" t="n">
-        <v>0.9398410896708286</v>
+        <v>0</v>
       </c>
       <c r="U140" s="8">
         <f>(T140-S140)/S140</f>
@@ -11465,13 +11465,13 @@
         <v/>
       </c>
       <c r="H141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K141" s="8">
         <f>(J141-I141)/I141</f>
@@ -11488,7 +11488,7 @@
         <v>1</v>
       </c>
       <c r="O141" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="P141" s="8">
         <f>(O141-N141)/N141</f>
@@ -11499,13 +11499,13 @@
         <v/>
       </c>
       <c r="R141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U141" s="8">
         <f>(T141-S141)/S141</f>
@@ -11653,10 +11653,10 @@
         <v/>
       </c>
       <c r="R143" s="12" t="n">
-        <v>0.5327188940092166</v>
+        <v>0</v>
       </c>
       <c r="S143" s="4" t="n">
-        <v>0.5935483870967742</v>
+        <v>0</v>
       </c>
       <c r="T143" s="8" t="n">
         <v>0</v>
@@ -11701,7 +11701,7 @@
         <v>1</v>
       </c>
       <c r="J144" t="n">
-        <v>0.2606635071090048</v>
+        <v>1</v>
       </c>
       <c r="K144" s="8">
         <f>(J144-I144)/I144</f>
@@ -11729,13 +11729,13 @@
         <v/>
       </c>
       <c r="R144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U144" s="8">
         <f>(T144-S144)/S144</f>
@@ -11771,13 +11771,13 @@
         <v/>
       </c>
       <c r="H145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K145" s="8">
         <f>(J145-I145)/I145</f>
@@ -11805,13 +11805,13 @@
         <v/>
       </c>
       <c r="R145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U145" s="8">
         <f>(T145-S145)/S145</f>
@@ -11847,10 +11847,10 @@
         <v/>
       </c>
       <c r="H146" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I146" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J146" s="6" t="n">
         <v>0</v>
@@ -11959,13 +11959,13 @@
         <v/>
       </c>
       <c r="R147" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S147" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T147" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U147" s="8">
         <f>(T147-S147)/S147</f>
@@ -12007,7 +12007,7 @@
         <v>1</v>
       </c>
       <c r="J148" t="n">
-        <v>0.1825396825396826</v>
+        <v>1</v>
       </c>
       <c r="K148" s="8">
         <f>(J148-I148)/I148</f>
@@ -12035,13 +12035,13 @@
         <v/>
       </c>
       <c r="R148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U148" s="8">
         <f>(T148-S148)/S148</f>
@@ -12077,13 +12077,13 @@
         <v/>
       </c>
       <c r="H149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K149" s="8">
         <f>(J149-I149)/I149</f>
@@ -12111,13 +12111,13 @@
         <v/>
       </c>
       <c r="R149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U149" s="8">
         <f>(T149-S149)/S149</f>
@@ -12153,10 +12153,10 @@
         <v/>
       </c>
       <c r="H150" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I150" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J150" s="6" t="n">
         <v>0</v>
@@ -12231,13 +12231,13 @@
         <v/>
       </c>
       <c r="H151" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I151" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J151" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K151" s="8">
         <f>(J151-I151)/I151</f>
@@ -12265,13 +12265,13 @@
         <v/>
       </c>
       <c r="R151" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S151" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T151" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U151" s="8">
         <f>(T151-S151)/S151</f>
@@ -12313,7 +12313,7 @@
         <v>1</v>
       </c>
       <c r="J152" t="n">
-        <v>0.09090909090909094</v>
+        <v>1</v>
       </c>
       <c r="K152" s="8">
         <f>(J152-I152)/I152</f>
@@ -12341,13 +12341,13 @@
         <v/>
       </c>
       <c r="R152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U152" s="8">
         <f>(T152-S152)/S152</f>
@@ -12383,13 +12383,13 @@
         <v/>
       </c>
       <c r="H153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K153" s="8">
         <f>(J153-I153)/I153</f>
@@ -12417,13 +12417,13 @@
         <v/>
       </c>
       <c r="R153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U153" s="8">
         <f>(T153-S153)/S153</f>
@@ -12459,10 +12459,10 @@
         <v/>
       </c>
       <c r="H154" s="14" t="n">
-        <v>0</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="I154" s="5" t="n">
-        <v>0</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="J154" s="6" t="n">
         <v>0</v>
@@ -12537,13 +12537,13 @@
         <v/>
       </c>
       <c r="H155" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I155" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J155" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K155" s="8">
         <f>(J155-I155)/I155</f>
@@ -12571,13 +12571,13 @@
         <v/>
       </c>
       <c r="R155" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S155" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T155" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U155" s="8">
         <f>(T155-S155)/S155</f>
@@ -12619,7 +12619,7 @@
         <v>1</v>
       </c>
       <c r="J156" t="n">
-        <v>0.3846153846153869</v>
+        <v>1</v>
       </c>
       <c r="K156" s="8">
         <f>(J156-I156)/I156</f>
@@ -12647,13 +12647,13 @@
         <v/>
       </c>
       <c r="R156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U156" s="8">
         <f>(T156-S156)/S156</f>
@@ -12689,13 +12689,13 @@
         <v/>
       </c>
       <c r="H157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K157" s="8">
         <f>(J157-I157)/I157</f>
@@ -12723,13 +12723,13 @@
         <v/>
       </c>
       <c r="R157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U157" s="8">
         <f>(T157-S157)/S157</f>
@@ -12765,10 +12765,10 @@
         <v/>
       </c>
       <c r="H158" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I158" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J158" s="6" t="n">
         <v>0</v>
@@ -12843,13 +12843,13 @@
         <v/>
       </c>
       <c r="H159" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I159" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J159" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K159" s="8">
         <f>(J159-I159)/I159</f>
@@ -12877,13 +12877,13 @@
         <v/>
       </c>
       <c r="R159" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S159" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T159" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U159" s="8">
         <f>(T159-S159)/S159</f>
@@ -12925,7 +12925,7 @@
         <v>1</v>
       </c>
       <c r="J160" t="n">
-        <v>0.1636363636363637</v>
+        <v>1</v>
       </c>
       <c r="K160" s="8">
         <f>(J160-I160)/I160</f>
@@ -12953,13 +12953,13 @@
         <v/>
       </c>
       <c r="R160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U160" s="8">
         <f>(T160-S160)/S160</f>
@@ -12995,13 +12995,13 @@
         <v/>
       </c>
       <c r="H161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K161" s="8">
         <f>(J161-I161)/I161</f>
@@ -13029,13 +13029,13 @@
         <v/>
       </c>
       <c r="R161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U161" s="8">
         <f>(T161-S161)/S161</f>
@@ -13149,13 +13149,13 @@
         <v/>
       </c>
       <c r="H163" s="12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I163" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J163" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K163" s="8">
         <f>(J163-I163)/I163</f>
@@ -13183,13 +13183,13 @@
         <v/>
       </c>
       <c r="R163" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S163" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T163" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U163" s="8">
         <f>(T163-S163)/S163</f>
@@ -13231,7 +13231,7 @@
         <v>1</v>
       </c>
       <c r="J164" t="n">
-        <v>0.3815028901734104</v>
+        <v>1</v>
       </c>
       <c r="K164" s="8">
         <f>(J164-I164)/I164</f>
@@ -13259,13 +13259,13 @@
         <v/>
       </c>
       <c r="R164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U164" s="8">
         <f>(T164-S164)/S164</f>
@@ -13301,13 +13301,13 @@
         <v/>
       </c>
       <c r="H165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K165" s="8">
         <f>(J165-I165)/I165</f>
@@ -13335,13 +13335,13 @@
         <v/>
       </c>
       <c r="R165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U165" s="8">
         <f>(T165-S165)/S165</f>

</xml_diff>